<commit_message>
edits to solve github issues
</commit_message>
<xml_diff>
--- a/excel2sbol/tests/test_files/pichia_comb_dev_compiler_sbol3_v003.xlsx
+++ b/excel2sbol/tests/test_files/pichia_comb_dev_compiler_sbol3_v003.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="9700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="9700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="9" r:id="rId1"/>
@@ -23481,43 +23481,6 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -23808,6 +23771,23 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="0"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -23870,6 +23850,26 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -23948,25 +23948,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:P28" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:P28" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:P28"/>
   <tableColumns count="16">
-    <tableColumn id="16" name="Sheet Name" dataDxfId="22"/>
-    <tableColumn id="1" name="Column Name" dataDxfId="21"/>
+    <tableColumn id="16" name="Sheet Name" dataDxfId="20"/>
+    <tableColumn id="1" name="Column Name" dataDxfId="19"/>
     <tableColumn id="2" name="SBOL Term"/>
-    <tableColumn id="3" name="Namespace URL" dataDxfId="20"/>
-    <tableColumn id="17" name="Type" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Namespace URL" dataDxfId="18"/>
+    <tableColumn id="17" name="Type" dataDxfId="17" dataCellStyle="Hyperlink"/>
     <tableColumn id="4" name="Split On"/>
     <tableColumn id="6" name="Pattern"/>
-    <tableColumn id="7" name="Tyto Lookup" dataDxfId="19"/>
-    <tableColumn id="8" name="Sheet Lookup" dataDxfId="18"/>
-    <tableColumn id="9" name="Replacement Lookup" dataDxfId="17"/>
-    <tableColumn id="10" name="Object_ID Lookup" dataDxfId="16"/>
-    <tableColumn id="11" name="Parent Lookup" dataDxfId="15"/>
-    <tableColumn id="12" name="Lookup Sheet Name" dataDxfId="14"/>
-    <tableColumn id="13" name="From Col" dataDxfId="13"/>
-    <tableColumn id="14" name="To Col" dataDxfId="12"/>
-    <tableColumn id="15" name="Ontology Name" dataDxfId="11"/>
+    <tableColumn id="7" name="Tyto Lookup" dataDxfId="16"/>
+    <tableColumn id="8" name="Sheet Lookup" dataDxfId="15"/>
+    <tableColumn id="9" name="Replacement Lookup" dataDxfId="14"/>
+    <tableColumn id="10" name="Object_ID Lookup" dataDxfId="13"/>
+    <tableColumn id="11" name="Parent Lookup" dataDxfId="12"/>
+    <tableColumn id="12" name="Lookup Sheet Name" dataDxfId="11"/>
+    <tableColumn id="13" name="From Col" dataDxfId="10"/>
+    <tableColumn id="14" name="To Col" dataDxfId="9"/>
+    <tableColumn id="15" name="Ontology Name" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -23976,11 +23976,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table_14" displayName="Table_14" ref="A19:I21">
   <tableColumns count="9">
     <tableColumn id="1" name="Collection Name"/>
-    <tableColumn id="16" name="SBOL Object Type" dataDxfId="10"/>
-    <tableColumn id="15" name="Thing1" dataDxfId="9"/>
+    <tableColumn id="16" name="SBOL Object Type" dataDxfId="7"/>
+    <tableColumn id="15" name="Thing1" dataDxfId="6"/>
     <tableColumn id="5" name="Description"/>
     <tableColumn id="6" name="Data Source Prefix"/>
-    <tableColumn id="7" name="Data Source" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="Data Source" dataDxfId="5" dataCellStyle="Normal"/>
     <tableColumn id="8" name="Source Organism"/>
     <tableColumn id="9" name="Target Organism"/>
     <tableColumn id="13" name="Data Source Composite">
@@ -23995,17 +23995,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A19:P27">
   <tableColumns count="16">
     <tableColumn id="1" name="Part Name"/>
-    <tableColumn id="11" name="Collection" dataDxfId="7"/>
-    <tableColumn id="16" name="SBOL Object Type" dataDxfId="6"/>
-    <tableColumn id="12" name="Molecule Type" dataDxfId="5"/>
+    <tableColumn id="11" name="Collection" dataDxfId="4"/>
+    <tableColumn id="16" name="SBOL Object Type" dataDxfId="3"/>
+    <tableColumn id="12" name="Molecule Type" dataDxfId="2"/>
     <tableColumn id="2" name="Role"/>
-    <tableColumn id="15" name="Thing1" dataDxfId="4"/>
+    <tableColumn id="15" name="Thing1" dataDxfId="1"/>
     <tableColumn id="14" name="SubComponents" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" name="Design Notes"/>
     <tableColumn id="4" name="Altered Sequence"/>
     <tableColumn id="5" name="Part Description"/>
     <tableColumn id="6" name="Data Source Prefix"/>
-    <tableColumn id="7" name="Data Source" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="Data Source" dataDxfId="0" dataCellStyle="Normal"/>
     <tableColumn id="8" name="Source Organism"/>
     <tableColumn id="9" name="Target Organism"/>
     <tableColumn id="10" name="Circular"/>
@@ -25745,11 +25745,11 @@
   </sheetPr>
   <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -26975,10 +26975,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:L28">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27011,7 +27011,7 @@
   <dimension ref="A1:Z90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -27802,8 +27802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>